<commit_message>
Revisión 23 de marzo coordinadora
Pendiente preguntas a la editora
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado11/guion09/SolicitudGrafica_CN_11_09_REC_90.xlsx
+++ b/fuentes/contenidos/grado11/guion09/SolicitudGrafica_CN_11_09_REC_90.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LyzMarcela\Documents\GitHub\CienciasNaturales\fuentes\contenidos\grado11\guion09\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8955" tabRatio="500"/>
   </bookViews>
@@ -752,7 +747,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="36">
+  <borders count="37">
     <border>
       <left/>
       <right/>
@@ -1197,6 +1192,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1251,7 +1259,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="116">
+  <cellXfs count="118">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1562,6 +1570,12 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="51">
@@ -1679,7 +1693,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp4.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="16" dropStyle="combo" dx="33" fmlaLink="$K$44" fmlaRange="$K$4:$K$43" noThreeD="1" sel="1" val="0"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="16" dropStyle="combo" dx="33" fmlaLink="$K$44" fmlaRange="$K$4:$K$43" noThreeD="1" val="0"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp5.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1888,7 +1902,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1896,20 +1910,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:noFill/>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1943,7 +1943,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1951,20 +1951,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:noFill/>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1998,7 +1984,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2006,20 +1992,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:noFill/>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2053,7 +2025,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2061,20 +2033,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:noFill/>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2108,7 +2066,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2116,20 +2074,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:noFill/>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2163,7 +2107,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2171,20 +2115,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:noFill/>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2218,7 +2148,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2226,20 +2156,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:noFill/>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2577,7 +2493,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="140" workbookViewId="0">
       <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
+      <selection pane="bottomLeft" activeCell="C3" sqref="C3:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -2632,10 +2548,10 @@
       <c r="B3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="94">
+      <c r="C3" s="116">
         <v>11</v>
       </c>
-      <c r="D3" s="95"/>
+      <c r="D3" s="117"/>
       <c r="F3" s="87"/>
       <c r="G3" s="88"/>
       <c r="H3" s="55"/>

</xml_diff>